<commit_message>
Revision of first 3 examples (DD-based recipes)
</commit_message>
<xml_diff>
--- a/examples/example_01/data/input.xlsx
+++ b/examples/example_01/data/input.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olgpao\Desktop\Github\CreateDaysOfTreatment\examples\example_01\input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olgpao\Desktop\Github\CreateDaysOfTreatment\examples\example_01\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15530" windowHeight="7050"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15525" windowHeight="7050"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -505,15 +505,15 @@
   <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:13" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -554,7 +554,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:13" ht="39" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>10</v>
       </c>
@@ -587,7 +587,7 @@
       <c r="L2" s="6"/>
       <c r="M2" s="6"/>
     </row>
-    <row r="3" spans="1:13" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:13" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>13</v>
       </c>
@@ -595,7 +595,7 @@
         <v>2</v>
       </c>
       <c r="C3" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D3" s="6" t="s">
         <v>14</v>

</xml_diff>